<commit_message>
Adding reading and recording
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\java-read-write-excel-file-using-apache-poi-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\Тех.задания для трудоустройства\testworkingwithexcel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEB643-2C9B-42AD-AB21-BD24E68E44B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59724F5A-C991-424A-B3EC-E5D847416BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="180" windowWidth="12396" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="876" yWindow="600" windowWidth="12396" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" r:id="rId1"/>
@@ -30,40 +30,40 @@
     <t/>
   </si>
   <si>
-    <t>workersCount</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>maxWorkersCount</t>
+  </si>
+  <si>
+    <t>sourceCenter</t>
+  </si>
+  <si>
+    <t>destCenter</t>
+  </si>
+  <si>
+    <t>Производственный центр №1</t>
+  </si>
+  <si>
+    <t>Производственный центр №2</t>
+  </si>
+  <si>
+    <t>Производственный центр №3</t>
+  </si>
+  <si>
+    <t>Производственный центр №4</t>
+  </si>
+  <si>
+    <t>Производственный центр №5</t>
+  </si>
+  <si>
+    <t>performance</t>
   </si>
   <si>
     <t>detailsCount</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>performance</t>
-  </si>
-  <si>
-    <t>maxWorkersCount</t>
-  </si>
-  <si>
-    <t>sourceCenter</t>
-  </si>
-  <si>
-    <t>destCenter</t>
-  </si>
-  <si>
-    <t>Производственный центр №1</t>
-  </si>
-  <si>
-    <t>Производственный центр №2</t>
-  </si>
-  <si>
-    <t>Производственный центр №3</t>
-  </si>
-  <si>
-    <t>Производственный центр №4</t>
-  </si>
-  <si>
-    <t>Производственный центр №5</t>
+    <t>workerCount</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -121,6 +121,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -404,9 +405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,11 +424,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
+      <c r="A2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -450,7 +451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A7"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,26 +477,26 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6">
         <v>2.2000000000000002</v>
       </c>
       <c r="D3" s="2">
@@ -504,12 +505,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
         <v>3.5</v>
       </c>
       <c r="D4" s="2">
@@ -518,12 +519,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
         <v>3</v>
       </c>
       <c r="D5" s="2">
@@ -532,12 +533,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6">
         <v>1.5</v>
       </c>
       <c r="D6" s="2">
@@ -546,12 +547,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="2">
@@ -568,9 +569,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="A2:B7"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,50 +589,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing code without multi plate
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\Тех.задания для трудоустройства\testworkingwithexcel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59724F5A-C991-424A-B3EC-E5D847416BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889FAF40-C2C4-4815-A0EE-ACB30DD55A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="876" yWindow="600" windowWidth="12396" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -64,6 +64,51 @@
   </si>
   <si>
     <t>workerCount</t>
+  </si>
+  <si>
+    <t>Производственный центр №6</t>
+  </si>
+  <si>
+    <t>Производственный центр №7</t>
+  </si>
+  <si>
+    <t>Производственный центр №8</t>
+  </si>
+  <si>
+    <t>Производственный центр №9</t>
+  </si>
+  <si>
+    <t>Производственный центр №10</t>
+  </si>
+  <si>
+    <t>Производственный центр №11</t>
+  </si>
+  <si>
+    <t>Производственный центр №12</t>
+  </si>
+  <si>
+    <t>Производственный центр №13</t>
+  </si>
+  <si>
+    <t>Производственный центр №14</t>
+  </si>
+  <si>
+    <t>Производственный центр №15</t>
+  </si>
+  <si>
+    <t>Производственный центр №16</t>
+  </si>
+  <si>
+    <t>Производственный центр №17</t>
+  </si>
+  <si>
+    <t>Производственный центр №18</t>
+  </si>
+  <si>
+    <t>Производственный центр №19</t>
+  </si>
+  <si>
+    <t>Производственный центр №20</t>
   </si>
 </sst>
 </file>
@@ -407,7 +452,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,10 +478,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -447,16 +492,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C7"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
@@ -497,10 +543,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>2.2000000000000002</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -514,7 +560,7 @@
         <v>3.5</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -542,7 +588,7 @@
         <v>1.5</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -556,7 +602,217 @@
         <v>1</v>
       </c>
       <c r="D7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="6">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -567,11 +823,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,23 +861,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -629,10 +885,138 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>